<commit_message>
changes email and home link format and position
</commit_message>
<xml_diff>
--- a/03-output/MSFT_stock.xlsx
+++ b/03-output/MSFT_stock.xlsx
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>250.4048762525634</v>
+        <v>250.404860853483</v>
       </c>
       <c r="D30" t="n">
-        <v>250.7619463067842</v>
+        <v>250.7619308857453</v>
       </c>
       <c r="E30" t="n">
-        <v>247.3598600770439</v>
+        <v>247.3598448652222</v>
       </c>
       <c r="F30" t="n">
-        <v>248.1235961914062</v>
+        <v>248.1235809326172</v>
       </c>
       <c r="G30" t="n">
         <v>21190000</v>
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>247.0424761430475</v>
+        <v>247.0424456682922</v>
       </c>
       <c r="D31" t="n">
-        <v>249.4427745424436</v>
+        <v>249.4427437715914</v>
       </c>
       <c r="E31" t="n">
-        <v>246.7052323790813</v>
+        <v>246.7052019459279</v>
       </c>
       <c r="F31" t="n">
-        <v>247.3896179199219</v>
+        <v>247.3895874023438</v>
       </c>
       <c r="G31" t="n">
         <v>22491000</v>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>250.137051855551</v>
+        <v>250.1370669290523</v>
       </c>
       <c r="D34" t="n">
-        <v>253.5391227049115</v>
+        <v>253.5391379834249</v>
       </c>
       <c r="E34" t="n">
-        <v>249.3435612218823</v>
+        <v>249.3435762475671</v>
       </c>
       <c r="F34" t="n">
-        <v>253.2118072509766</v>
+        <v>253.2118225097656</v>
       </c>
       <c r="G34" t="n">
         <v>30760100</v>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>248.4112213134766</v>
+        <v>248.4112152099609</v>
       </c>
     </row>
     <row r="35">
@@ -701,16 +701,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>254.3425253196051</v>
+        <v>254.3425100869534</v>
       </c>
       <c r="D35" t="n">
-        <v>258.0024893105154</v>
+        <v>258.0024738586674</v>
       </c>
       <c r="E35" t="n">
-        <v>253.8961915697666</v>
+        <v>253.896176363846</v>
       </c>
       <c r="F35" t="n">
-        <v>254.7789459228516</v>
+        <v>254.7789306640625</v>
       </c>
       <c r="G35" t="n">
         <v>24109800</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>249.7422912597656</v>
+        <v>249.74228515625</v>
       </c>
     </row>
     <row r="36">
@@ -732,16 +732,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>254.2135770706134</v>
+        <v>254.2135924584848</v>
       </c>
       <c r="D36" t="n">
-        <v>255.5922763011622</v>
+        <v>255.5922917724881</v>
       </c>
       <c r="E36" t="n">
-        <v>251.3272774355169</v>
+        <v>251.327292648677</v>
       </c>
       <c r="F36" t="n">
-        <v>252.0810852050781</v>
+        <v>252.0811004638672</v>
       </c>
       <c r="G36" t="n">
         <v>21473200</v>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>250.6805847167969</v>
+        <v>250.6805877685547</v>
       </c>
     </row>
     <row r="37">
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>252.1544891357422</v>
+        <v>252.1544921875</v>
       </c>
     </row>
     <row r="38">
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>252.3945220947266</v>
+        <v>252.3945251464844</v>
       </c>
     </row>
     <row r="39">
@@ -825,16 +825,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>249.0360961872708</v>
+        <v>249.0360807756418</v>
       </c>
       <c r="D39" t="n">
-        <v>250.7321675325816</v>
+        <v>250.7321520159911</v>
       </c>
       <c r="E39" t="n">
-        <v>245.5844292109504</v>
+        <v>245.5844140129283</v>
       </c>
       <c r="F39" t="n">
-        <v>246.5663604736328</v>
+        <v>246.5663452148438</v>
       </c>
       <c r="G39" t="n">
         <v>28333900</v>
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>251.0654327392578</v>
+        <v>251.0654296875</v>
       </c>
     </row>
     <row r="40">
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>251.7974304199219</v>
+        <v>251.7974273681641</v>
       </c>
     </row>
     <row r="42">
@@ -918,16 +918,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>257.8636007937159</v>
+        <v>257.86363068356</v>
       </c>
       <c r="D42" t="n">
-        <v>264.310686470804</v>
+        <v>264.3107171079516</v>
       </c>
       <c r="E42" t="n">
-        <v>257.0998497335621</v>
+        <v>257.0998795348772</v>
       </c>
       <c r="F42" t="n">
-        <v>263.2791442871094</v>
+        <v>263.2791748046875</v>
       </c>
       <c r="G42" t="n">
         <v>46028000</v>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>254.1263061523437</v>
+        <v>254.1263092041016</v>
       </c>
     </row>
     <row r="43">
@@ -970,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>258.8634246826172</v>
+        <v>258.863427734375</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>264.9812133789063</v>
+        <v>264.9812194824219</v>
       </c>
     </row>
     <row r="45">
@@ -1011,16 +1011,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>274.7252795761171</v>
+        <v>274.7252485260536</v>
       </c>
       <c r="D45" t="n">
-        <v>275.2212093701081</v>
+        <v>275.2211782639934</v>
       </c>
       <c r="E45" t="n">
-        <v>267.6533158707418</v>
+        <v>267.6532856199674</v>
       </c>
       <c r="F45" t="n">
-        <v>270.0139465332031</v>
+        <v>270.013916015625</v>
       </c>
       <c r="G45" t="n">
         <v>43466600</v>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>272.54912109375</v>
+        <v>272.5491149902344</v>
       </c>
     </row>
     <row r="48">
@@ -1125,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>272.8387451171875</v>
+        <v>272.8387390136719</v>
       </c>
     </row>
     <row r="49">
@@ -1135,16 +1135,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>274.9831018515552</v>
+        <v>274.9831320069276</v>
       </c>
       <c r="D49" t="n">
-        <v>278.3455198871405</v>
+        <v>278.3455504112446</v>
       </c>
       <c r="E49" t="n">
-        <v>273.0390658217448</v>
+        <v>273.0390957639291</v>
       </c>
       <c r="F49" t="n">
-        <v>278.2860107421875</v>
+        <v>278.2860412597656</v>
       </c>
       <c r="G49" t="n">
         <v>28172000</v>
@@ -1159,10 +1159,10 @@
         <v>273.0648864746094</v>
       </c>
       <c r="K49" t="n">
-        <v>259.3806884765625</v>
+        <v>259.380687713623</v>
       </c>
       <c r="L49" t="n">
-        <v>278.21661412567</v>
+        <v>278.2165831531665</v>
       </c>
     </row>
     <row r="50">
@@ -1172,16 +1172,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>278.21661412567</v>
+        <v>278.2165831531665</v>
       </c>
       <c r="D50" t="n">
-        <v>279.168790853732</v>
+        <v>279.1687597752273</v>
       </c>
       <c r="E50" t="n">
-        <v>273.2771424860092</v>
+        <v>273.2771120633931</v>
       </c>
       <c r="F50" t="n">
-        <v>274.1301574707031</v>
+        <v>274.130126953125</v>
       </c>
       <c r="G50" t="n">
         <v>26840200</v>
@@ -1196,7 +1196,7 @@
         <v>273.8881286621094</v>
       </c>
       <c r="K50" t="n">
-        <v>260.6810165405274</v>
+        <v>260.6810150146484</v>
       </c>
     </row>
     <row r="51">
@@ -1206,16 +1206,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>273.5449714330365</v>
+        <v>273.5449408533657</v>
       </c>
       <c r="D51" t="n">
-        <v>273.8921283517831</v>
+        <v>273.8920977333036</v>
       </c>
       <c r="E51" t="n">
-        <v>269.8353958934812</v>
+        <v>269.8353657285049</v>
       </c>
       <c r="F51" t="n">
-        <v>272.9895324707031</v>
+        <v>272.989501953125</v>
       </c>
       <c r="G51" t="n">
         <v>21878600</v>
@@ -1227,10 +1227,10 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>274.1757751464844</v>
+        <v>274.1757690429687</v>
       </c>
       <c r="K51" t="n">
-        <v>261.9610122680664</v>
+        <v>261.9610107421875</v>
       </c>
     </row>
     <row r="52">
@@ -1240,16 +1240,16 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>276.6891011698945</v>
+        <v>276.6891315188411</v>
       </c>
       <c r="D52" t="n">
-        <v>278.851377755701</v>
+        <v>278.8514083418194</v>
       </c>
       <c r="E52" t="n">
-        <v>276.1435905850354</v>
+        <v>276.1436208741472</v>
       </c>
       <c r="F52" t="n">
-        <v>278.2265014648438</v>
+        <v>278.2265319824219</v>
       </c>
       <c r="G52" t="n">
         <v>25087000</v>
@@ -1274,16 +1274,16 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>281.9162591448602</v>
+        <v>281.9162286079409</v>
       </c>
       <c r="D53" t="n">
-        <v>282.1443674758609</v>
+        <v>282.144336914233</v>
       </c>
       <c r="E53" t="n">
-        <v>279.1886453015576</v>
+        <v>279.1886150600909</v>
       </c>
       <c r="F53" t="n">
-        <v>281.7377014160156</v>
+        <v>281.7376708984375</v>
       </c>
       <c r="G53" t="n">
         <v>25053400</v>
@@ -1295,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>277.0739807128906</v>
+        <v>277.073974609375</v>
       </c>
       <c r="K53" t="n">
-        <v>265.2926681518555</v>
+        <v>265.2926666259766</v>
       </c>
     </row>
     <row r="54">
@@ -1329,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>278.6073913574219</v>
+        <v>278.6073791503906</v>
       </c>
       <c r="K54" t="n">
-        <v>266.9297309875489</v>
+        <v>266.9297286987305</v>
       </c>
     </row>
     <row r="55">
@@ -1363,10 +1363,10 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>280.7597229003906</v>
+        <v>280.759716796875</v>
       </c>
       <c r="K55" t="n">
-        <v>268.4353744506836</v>
+        <v>268.4353729248047</v>
       </c>
     </row>
     <row r="56">
@@ -1400,7 +1400,7 @@
         <v>283.1302551269531</v>
       </c>
       <c r="K56" t="n">
-        <v>270.0734298706055</v>
+        <v>270.0734275817871</v>
       </c>
     </row>
     <row r="57">
@@ -1431,10 +1431,10 @@
         <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>283.8900207519531</v>
+        <v>283.8900146484375</v>
       </c>
       <c r="K57" t="n">
-        <v>271.5929580688477</v>
+        <v>271.5929557800293</v>
       </c>
     </row>
     <row r="58">
@@ -1444,16 +1444,16 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>280.9045113442665</v>
+        <v>280.9045409837825</v>
       </c>
       <c r="D58" t="n">
-        <v>289.7022999788345</v>
+        <v>289.7023305466453</v>
       </c>
       <c r="E58" t="n">
-        <v>279.7341244370916</v>
+        <v>279.7341539531147</v>
       </c>
       <c r="F58" t="n">
-        <v>289.2262268066406</v>
+        <v>289.2262573242188</v>
       </c>
       <c r="G58" t="n">
         <v>29770300</v>
@@ -1465,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>285.3877258300781</v>
+        <v>285.3877319335937</v>
       </c>
       <c r="K58" t="n">
-        <v>273.5409690856933</v>
+        <v>273.5409683227539</v>
       </c>
     </row>
     <row r="59">
@@ -1478,16 +1478,16 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>286.8556525060943</v>
+        <v>286.8556830046882</v>
       </c>
       <c r="D59" t="n">
-        <v>287.2424922065542</v>
+        <v>287.2425227462769</v>
       </c>
       <c r="E59" t="n">
-        <v>282.3922851452958</v>
+        <v>282.3923151693428</v>
       </c>
       <c r="F59" t="n">
-        <v>287.0342102050781</v>
+        <v>287.0342407226562</v>
       </c>
       <c r="G59" t="n">
         <v>23103000</v>
@@ -1499,10 +1499,10 @@
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>285.603955078125</v>
+        <v>285.6039672851563</v>
       </c>
       <c r="K59" t="n">
-        <v>275.5643615722656</v>
+        <v>275.5643630981446</v>
       </c>
     </row>
     <row r="60">
@@ -1533,10 +1533,10 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>284.7311157226562</v>
+        <v>284.7311279296875</v>
       </c>
       <c r="K60" t="n">
-        <v>276.9980941772461</v>
+        <v>276.998095703125</v>
       </c>
     </row>
     <row r="61">
@@ -1546,16 +1546,16 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>282.4716558810065</v>
+        <v>282.4716865385311</v>
       </c>
       <c r="D61" t="n">
-        <v>284.6735850289912</v>
+        <v>284.6736159254979</v>
       </c>
       <c r="E61" t="n">
-        <v>279.6646767400454</v>
+        <v>279.6647070929199</v>
       </c>
       <c r="F61" t="n">
-        <v>281.1822204589844</v>
+        <v>281.1822509765625</v>
       </c>
       <c r="G61" t="n">
         <v>27403400</v>
@@ -1567,10 +1567,10 @@
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>283.99912109375</v>
+        <v>283.9991394042969</v>
       </c>
       <c r="K61" t="n">
-        <v>278.1238525390625</v>
+        <v>278.1238555908203</v>
       </c>
     </row>
     <row r="62">
@@ -1601,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>285.0901611328125</v>
+        <v>285.0901794433594</v>
       </c>
       <c r="K62" t="n">
-        <v>279.3339218139648</v>
+        <v>279.3339233398438</v>
       </c>
     </row>
     <row r="63">
@@ -1614,16 +1614,16 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>284.6636841265514</v>
+        <v>284.6636535172536</v>
       </c>
       <c r="D63" t="n">
-        <v>286.1316471227742</v>
+        <v>286.1316163556294</v>
       </c>
       <c r="E63" t="n">
-        <v>281.3806315151257</v>
+        <v>281.3806012588477</v>
       </c>
       <c r="F63" t="n">
-        <v>283.8106994628906</v>
+        <v>283.8106689453125</v>
       </c>
       <c r="G63" t="n">
         <v>20987900</v>
@@ -1635,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>284.0070556640625</v>
+        <v>284.0070617675781</v>
       </c>
       <c r="K63" t="n">
         <v>279.8268768310547</v>
@@ -1682,16 +1682,16 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>289.1964845113955</v>
+        <v>289.1964536551669</v>
       </c>
       <c r="D65" t="n">
-        <v>289.3849402397728</v>
+        <v>289.3849093634367</v>
       </c>
       <c r="E65" t="n">
-        <v>284.6736075686396</v>
+        <v>284.6735771949859</v>
       </c>
       <c r="F65" t="n">
-        <v>286.0225219726562</v>
+        <v>286.0224914550781</v>
       </c>
       <c r="G65" t="n">
         <v>20161800</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>284.9890014648437</v>
+        <v>284.9889953613281</v>
       </c>
       <c r="K65" t="n">
         <v>281.0919921875</v>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>285.9729370117187</v>
+        <v>285.9729248046875</v>
       </c>
       <c r="K66" t="n">
         <v>281.8195220947266</v>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>285.2330139160156</v>
+        <v>285.2330017089844</v>
       </c>
       <c r="K67" t="n">
         <v>282.5048950195313</v>
@@ -1784,16 +1784,16 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>282.68991267727</v>
+        <v>282.6898822397877</v>
       </c>
       <c r="D68" t="n">
-        <v>283.9396351831513</v>
+        <v>283.9396046111103</v>
       </c>
       <c r="E68" t="n">
-        <v>280.7557743605892</v>
+        <v>280.7557441313573</v>
       </c>
       <c r="F68" t="n">
-        <v>283.4338073730469</v>
+        <v>283.4337768554688</v>
       </c>
       <c r="G68" t="n">
         <v>21676400</v>
@@ -1805,10 +1805,10 @@
         <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>285.1576354980469</v>
+        <v>285.1576232910156</v>
       </c>
       <c r="K68" t="n">
-        <v>282.9065994262695</v>
+        <v>282.9065979003906</v>
       </c>
     </row>
     <row r="69">
@@ -1818,16 +1818,16 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>279.793659648015</v>
+        <v>279.793629095778</v>
       </c>
       <c r="D69" t="n">
-        <v>282.630393729573</v>
+        <v>282.630362867577</v>
       </c>
       <c r="E69" t="n">
-        <v>276.4510977738803</v>
+        <v>276.4510675866363</v>
       </c>
       <c r="F69" t="n">
-        <v>279.4762573242188</v>
+        <v>279.4762268066406</v>
       </c>
       <c r="G69" t="n">
         <v>26611000</v>
@@ -1839,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>283.7630798339844</v>
+        <v>283.7630615234375</v>
       </c>
       <c r="K69" t="n">
-        <v>282.9661117553711</v>
+        <v>282.9661071777344</v>
       </c>
     </row>
     <row r="70">
@@ -1873,16 +1873,16 @@
         <v>0</v>
       </c>
       <c r="J70" t="n">
-        <v>281.1941650390625</v>
+        <v>281.1941528320312</v>
       </c>
       <c r="K70" t="n">
-        <v>282.9185012817383</v>
+        <v>282.9184982299805</v>
       </c>
       <c r="M70" t="n">
-        <v>294.2847357849702</v>
+        <v>294.2847664399654</v>
       </c>
       <c r="N70" t="n">
-        <v>16.06812165930017</v>
+        <v>16.06818328679896</v>
       </c>
       <c r="O70" t="n">
         <v>21</v>
@@ -1895,16 +1895,16 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>294.2847357849702</v>
+        <v>294.2847664399654</v>
       </c>
       <c r="D71" t="n">
-        <v>297.131367803901</v>
+        <v>297.1313987554236</v>
       </c>
       <c r="E71" t="n">
-        <v>290.3470522250336</v>
+        <v>290.3470824698489</v>
       </c>
       <c r="F71" t="n">
-        <v>292.9655456542969</v>
+        <v>292.965576171875</v>
       </c>
       <c r="G71" t="n">
         <v>64599200</v>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>282.56689453125</v>
+        <v>282.5668884277344</v>
       </c>
       <c r="K71" t="n">
         <v>283.917301940918</v>
@@ -1929,16 +1929,16 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>293.5606799448396</v>
+        <v>293.5606503142652</v>
       </c>
       <c r="D72" t="n">
-        <v>302.7155547290051</v>
+        <v>302.7155241743824</v>
       </c>
       <c r="E72" t="n">
-        <v>292.8465398392919</v>
+        <v>292.8465102807992</v>
       </c>
       <c r="F72" t="n">
-        <v>302.3485412597656</v>
+        <v>302.3485107421875</v>
       </c>
       <c r="G72" t="n">
         <v>46462600</v>
@@ -1950,10 +1950,10 @@
         <v>0</v>
       </c>
       <c r="J72" t="n">
-        <v>286.280419921875</v>
+        <v>286.2804077148438</v>
       </c>
       <c r="K72" t="n">
-        <v>285.123403930664</v>
+        <v>285.1234008789062</v>
       </c>
       <c r="L72" t="n">
         <v>301.5352453764582</v>
@@ -1987,10 +1987,10 @@
         <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>290.5454162597656</v>
+        <v>290.54541015625</v>
       </c>
       <c r="K73" t="n">
-        <v>286.2744583129883</v>
+        <v>286.2744567871094</v>
       </c>
     </row>
     <row r="74">
@@ -2000,16 +2000,16 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>304.471126914505</v>
+        <v>304.4710962561039</v>
       </c>
       <c r="D74" t="n">
-        <v>306.0878628221589</v>
+        <v>306.0878320009622</v>
       </c>
       <c r="E74" t="n">
-        <v>302.6659352710417</v>
+        <v>302.6659047944124</v>
       </c>
       <c r="F74" t="n">
-        <v>303.0726013183594</v>
+        <v>303.0725708007812</v>
       </c>
       <c r="G74" t="n">
         <v>21294100</v>
@@ -2021,10 +2021,10 @@
         <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>295.2646850585937</v>
+        <v>295.2646789550781</v>
       </c>
       <c r="K74" t="n">
-        <v>287.1304351806641</v>
+        <v>287.1304321289062</v>
       </c>
     </row>
     <row r="75">
@@ -2055,10 +2055,10 @@
         <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>301.2138549804687</v>
+        <v>301.2138488769531</v>
       </c>
       <c r="K75" t="n">
-        <v>288.0320343017578</v>
+        <v>288.03203125</v>
       </c>
     </row>
     <row r="76">
@@ -2089,10 +2089,10 @@
         <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>303.0051574707031</v>
+        <v>303.0051452636719</v>
       </c>
       <c r="K76" t="n">
-        <v>288.8860275268555</v>
+        <v>288.8860244750977</v>
       </c>
     </row>
     <row r="77">
@@ -2123,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>303.1202087402344</v>
+        <v>303.1202026367188</v>
       </c>
       <c r="K77" t="n">
-        <v>289.9309509277344</v>
+        <v>289.9309478759766</v>
       </c>
     </row>
     <row r="78">
@@ -2136,16 +2136,16 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>303.2312645677939</v>
+        <v>303.2313246343267</v>
       </c>
       <c r="D78" t="n">
-        <v>309.4303859729405</v>
+        <v>309.430447267446</v>
       </c>
       <c r="E78" t="n">
-        <v>301.7930562941409</v>
+        <v>301.7931160757815</v>
       </c>
       <c r="F78" t="n">
-        <v>308.1211242675781</v>
+        <v>308.1211853027344</v>
       </c>
       <c r="G78" t="n">
         <v>28181200</v>
@@ -2157,10 +2157,10 @@
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>303.79267578125</v>
+        <v>303.7926818847656</v>
       </c>
       <c r="K78" t="n">
-        <v>290.8756958007813</v>
+        <v>290.8756942749023</v>
       </c>
     </row>
     <row r="79">
@@ -2170,16 +2170,16 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>307.605414236902</v>
+        <v>307.6053529090755</v>
       </c>
       <c r="D79" t="n">
-        <v>307.6748516716129</v>
+        <v>307.6747903299425</v>
       </c>
       <c r="E79" t="n">
-        <v>303.5982930863674</v>
+        <v>303.5982325574476</v>
       </c>
       <c r="F79" t="n">
-        <v>306.137451171875</v>
+        <v>306.1373901367188</v>
       </c>
       <c r="G79" t="n">
         <v>21318600</v>
@@ -2194,7 +2194,7 @@
         <v>304.4056457519531</v>
       </c>
       <c r="K79" t="n">
-        <v>291.8308578491211</v>
+        <v>291.8308517456055</v>
       </c>
     </row>
     <row r="80">
@@ -2204,16 +2204,16 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>305.4927445700581</v>
+        <v>305.4927139530741</v>
       </c>
       <c r="D80" t="n">
-        <v>307.5161465484169</v>
+        <v>307.5161157286444</v>
       </c>
       <c r="E80" t="n">
-        <v>303.8164994916318</v>
+        <v>303.8164690426439</v>
       </c>
       <c r="F80" t="n">
-        <v>304.5008850097656</v>
+        <v>304.5008544921875</v>
       </c>
       <c r="G80" t="n">
         <v>21340800</v>
@@ -2225,10 +2225,10 @@
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>304.7210632324219</v>
+        <v>304.7210571289062</v>
       </c>
       <c r="K80" t="n">
-        <v>293.0295211791992</v>
+        <v>293.0295135498047</v>
       </c>
     </row>
     <row r="81">
@@ -2259,10 +2259,10 @@
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>306.2901794433594</v>
+        <v>306.2901733398438</v>
       </c>
       <c r="K81" t="n">
-        <v>294.4587921142578</v>
+        <v>294.4587829589844</v>
       </c>
     </row>
     <row r="82">
@@ -2272,16 +2272,16 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>307.575642759321</v>
+        <v>307.5756122427249</v>
       </c>
       <c r="D82" t="n">
-        <v>308.5873285713582</v>
+        <v>308.5872979543861</v>
       </c>
       <c r="E82" t="n">
-        <v>303.7669058403482</v>
+        <v>303.7668757016419</v>
       </c>
       <c r="F82" t="n">
-        <v>307.5855407714844</v>
+        <v>307.5855102539062</v>
       </c>
       <c r="G82" t="n">
         <v>31680200</v>
@@ -2293,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>307.2225280761719</v>
+        <v>307.2225158691406</v>
       </c>
       <c r="K82" t="n">
-        <v>295.4640426635742</v>
+        <v>295.4640319824219</v>
       </c>
     </row>
     <row r="83">
@@ -2327,10 +2327,10 @@
         <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>306.8892700195312</v>
+        <v>306.8892456054688</v>
       </c>
       <c r="K83" t="n">
-        <v>296.5962493896484</v>
+        <v>296.596240234375</v>
       </c>
     </row>
     <row r="84">
@@ -2340,16 +2340,16 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>306.5837715321622</v>
+        <v>306.5838020142402</v>
       </c>
       <c r="D84" t="n">
-        <v>307.377247009047</v>
+        <v>307.3772775700162</v>
       </c>
       <c r="E84" t="n">
-        <v>305.086054030207</v>
+        <v>305.0860843633745</v>
       </c>
       <c r="F84" t="n">
-        <v>306.9408264160156</v>
+        <v>306.9408569335938</v>
       </c>
       <c r="G84" t="n">
         <v>16336500</v>
@@ -2361,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>307.0499450683594</v>
+        <v>307.0499389648438</v>
       </c>
       <c r="K84" t="n">
-        <v>297.6208389282227</v>
+        <v>297.6208312988281</v>
       </c>
     </row>
     <row r="85">
@@ -2374,16 +2374,16 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>307.3078152325735</v>
+        <v>307.3078455631731</v>
       </c>
       <c r="D85" t="n">
-        <v>311.1562349314548</v>
+        <v>311.1562656418849</v>
       </c>
       <c r="E85" t="n">
-        <v>307.3078152325735</v>
+        <v>307.3078455631731</v>
       </c>
       <c r="F85" t="n">
-        <v>309.2022705078125</v>
+        <v>309.2023010253906</v>
       </c>
       <c r="G85" t="n">
         <v>26730300</v>
@@ -2395,10 +2395,10 @@
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>307.9902221679687</v>
+        <v>307.9902282714844</v>
       </c>
       <c r="K85" t="n">
-        <v>298.7798263549805</v>
+        <v>298.7798217773437</v>
       </c>
     </row>
     <row r="86">
@@ -2429,10 +2429,10 @@
         <v>0</v>
       </c>
       <c r="J86" t="n">
-        <v>308.4616394042969</v>
+        <v>308.4616455078125</v>
       </c>
       <c r="K86" t="n">
-        <v>300.0809677124024</v>
+        <v>300.0809631347656</v>
       </c>
     </row>
     <row r="87">
@@ -2442,16 +2442,16 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>312.6515754403516</v>
+        <v>312.6515453050567</v>
       </c>
       <c r="D87" t="n">
-        <v>317.1346507080416</v>
+        <v>317.1346201406401</v>
       </c>
       <c r="E87" t="n">
-        <v>311.8464153164205</v>
+        <v>311.846385258732</v>
       </c>
       <c r="F87" t="n">
-        <v>316.6177368164062</v>
+        <v>316.6177062988281</v>
       </c>
       <c r="G87" t="n">
         <v>27276000</v>
@@ -2463,10 +2463,10 @@
         <v>0</v>
       </c>
       <c r="J87" t="n">
-        <v>310.2680786132813</v>
+        <v>310.2680847167969</v>
       </c>
       <c r="K87" t="n">
-        <v>301.7228088378906</v>
+        <v>301.722802734375</v>
       </c>
     </row>
     <row r="88">
@@ -2497,10 +2497,10 @@
         <v>0</v>
       </c>
       <c r="J88" t="n">
-        <v>312.2648681640625</v>
+        <v>312.2648742675781</v>
       </c>
       <c r="K88" t="n">
-        <v>303.3730575561523</v>
+        <v>303.3730529785156</v>
       </c>
     </row>
     <row r="89">
@@ -2510,16 +2510,16 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>316.6972624495025</v>
+        <v>316.6972927219379</v>
       </c>
       <c r="D89" t="n">
-        <v>320.6634236554639</v>
+        <v>320.6634543070164</v>
       </c>
       <c r="E89" t="n">
-        <v>316.1107896890329</v>
+        <v>316.1108199054085</v>
       </c>
       <c r="F89" t="n">
-        <v>319.2618408203125</v>
+        <v>319.2618713378906</v>
       </c>
       <c r="G89" t="n">
         <v>24115700</v>
@@ -2531,10 +2531,10 @@
         <v>0</v>
       </c>
       <c r="J89" t="n">
-        <v>314.7290710449219</v>
+        <v>314.7290771484375</v>
       </c>
       <c r="K89" t="n">
-        <v>305.3623367309571</v>
+        <v>305.3623352050781</v>
       </c>
     </row>
     <row r="90">
@@ -2544,16 +2544,16 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>318.1186986986916</v>
+        <v>318.1187296780109</v>
       </c>
       <c r="D90" t="n">
-        <v>320.7926357652809</v>
+        <v>320.7926670049958</v>
       </c>
       <c r="E90" t="n">
-        <v>313.3672472808515</v>
+        <v>313.3672777974607</v>
       </c>
       <c r="F90" t="n">
-        <v>313.377197265625</v>
+        <v>313.3772277832031</v>
       </c>
       <c r="G90" t="n">
         <v>30797200</v>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>315.5640563964844</v>
+        <v>315.5640625</v>
       </c>
       <c r="K90" t="n">
         <v>307.3722991943359</v>
@@ -2599,10 +2599,10 @@
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>315.5342346191406</v>
+        <v>315.5342407226562</v>
       </c>
       <c r="K91" t="n">
-        <v>308.322802734375</v>
+        <v>308.3228012084961</v>
       </c>
     </row>
     <row r="92">
@@ -2612,16 +2612,16 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>321.3095540716889</v>
+        <v>321.3095238050552</v>
       </c>
       <c r="D92" t="n">
-        <v>324.9476996604213</v>
+        <v>324.9476690510825</v>
       </c>
       <c r="E92" t="n">
-        <v>318.0889135295059</v>
+        <v>318.0888835662493</v>
       </c>
       <c r="F92" t="n">
-        <v>323.9735717773438</v>
+        <v>323.9735412597656</v>
       </c>
       <c r="G92" t="n">
         <v>43301700</v>
@@ -2633,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="J92" t="n">
-        <v>317.0054016113281</v>
+        <v>317.0054077148437</v>
       </c>
       <c r="K92" t="n">
-        <v>309.4040542602539</v>
+        <v>309.404052734375</v>
       </c>
     </row>
     <row r="93">
@@ -2646,16 +2646,16 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>322.0848647666156</v>
+        <v>322.084835062194</v>
       </c>
       <c r="D93" t="n">
-        <v>331.4088500348929</v>
+        <v>331.4088194705626</v>
       </c>
       <c r="E93" t="n">
-        <v>321.9457166541965</v>
+        <v>321.9456869626079</v>
       </c>
       <c r="F93" t="n">
-        <v>330.9019165039062</v>
+        <v>330.9018859863281</v>
       </c>
       <c r="G93" t="n">
         <v>36630600</v>
@@ -2670,7 +2670,7 @@
         <v>319.8980285644531</v>
       </c>
       <c r="K93" t="n">
-        <v>310.7112106323242</v>
+        <v>310.7112075805664</v>
       </c>
     </row>
     <row r="94">
@@ -2701,10 +2701,10 @@
         <v>0</v>
       </c>
       <c r="J94" t="n">
-        <v>321.8920532226563</v>
+        <v>321.8920471191406</v>
       </c>
       <c r="K94" t="n">
-        <v>312.0191787719726</v>
+        <v>312.0191772460938</v>
       </c>
     </row>
     <row r="95">
@@ -2735,10 +2735,10 @@
         <v>0</v>
       </c>
       <c r="J95" t="n">
-        <v>324.5023742675781</v>
+        <v>324.5023620605469</v>
       </c>
       <c r="K95" t="n">
-        <v>313.1944290161133</v>
+        <v>313.1944274902344</v>
       </c>
     </row>
     <row r="96">
@@ -2769,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>328.2260009765625</v>
+        <v>328.2259887695312</v>
       </c>
       <c r="K96" t="n">
-        <v>314.6280136108398</v>
+        <v>314.6280120849609</v>
       </c>
     </row>
     <row r="97">
@@ -2782,16 +2782,16 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>332.253785740211</v>
+        <v>332.2538161531527</v>
       </c>
       <c r="D97" t="n">
-        <v>335.4843760278869</v>
+        <v>335.4844067365416</v>
       </c>
       <c r="E97" t="n">
-        <v>330.563926378683</v>
+        <v>330.5639566369431</v>
       </c>
       <c r="F97" t="n">
-        <v>333.3969116210938</v>
+        <v>333.3969421386719</v>
       </c>
       <c r="G97" t="n">
         <v>25864000</v>
@@ -2837,10 +2837,10 @@
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>330.7170288085937</v>
+        <v>330.7170349121094</v>
       </c>
       <c r="K98" t="n">
-        <v>317.4422988891602</v>
+        <v>317.4422958374024</v>
       </c>
     </row>
     <row r="99">
@@ -2871,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>331.2080749511719</v>
+        <v>331.2080810546875</v>
       </c>
       <c r="K99" t="n">
         <v>318.7197860717773</v>
@@ -2884,16 +2884,16 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>329.669298556267</v>
+        <v>329.6693298542892</v>
       </c>
       <c r="D100" t="n">
-        <v>332.4923337374677</v>
+        <v>332.4923653035022</v>
       </c>
       <c r="E100" t="n">
-        <v>320.5739506739762</v>
+        <v>320.5739811085077</v>
       </c>
       <c r="F100" t="n">
-        <v>321.4486999511719</v>
+        <v>321.44873046875</v>
       </c>
       <c r="G100" t="n">
         <v>40717100</v>
@@ -2905,10 +2905,10 @@
         <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>330.2120544433594</v>
+        <v>330.2120666503906</v>
       </c>
       <c r="K100" t="n">
-        <v>319.5671768188477</v>
+        <v>319.5671798706055</v>
       </c>
     </row>
     <row r="101">
@@ -2939,10 +2939,10 @@
         <v>0</v>
       </c>
       <c r="J101" t="n">
-        <v>328.7568054199219</v>
+        <v>328.7568176269531</v>
       </c>
       <c r="K101" t="n">
-        <v>320.2446701049805</v>
+        <v>320.2446731567383</v>
       </c>
     </row>
     <row r="102">
@@ -2973,10 +2973,10 @@
         <v>0</v>
       </c>
       <c r="J102" t="n">
-        <v>327.0450927734375</v>
+        <v>327.0450988769531</v>
       </c>
       <c r="K102" t="n">
-        <v>321.1073104858398</v>
+        <v>321.1073150634766</v>
       </c>
     </row>
     <row r="103">
@@ -2986,16 +2986,16 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>326.617643204137</v>
+        <v>326.6176129872763</v>
       </c>
       <c r="D103" t="n">
-        <v>330.1166404964646</v>
+        <v>330.116609955896</v>
       </c>
       <c r="E103" t="n">
-        <v>323.218085094812</v>
+        <v>323.2180551924596</v>
       </c>
       <c r="F103" t="n">
-        <v>329.8681335449219</v>
+        <v>329.8681030273438</v>
       </c>
       <c r="G103" t="n">
         <v>24260300</v>
@@ -3010,7 +3010,7 @@
         <v>326.2319763183594</v>
       </c>
       <c r="K103" t="n">
-        <v>322.2779754638672</v>
+        <v>322.277978515625</v>
       </c>
     </row>
     <row r="104">
@@ -3020,16 +3020,16 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>332.4724663004151</v>
+        <v>332.4724968344249</v>
       </c>
       <c r="D104" t="n">
-        <v>334.9674856868169</v>
+        <v>334.9675164499673</v>
       </c>
       <c r="E104" t="n">
-        <v>328.4168463847186</v>
+        <v>328.4168765462634</v>
       </c>
       <c r="F104" t="n">
-        <v>332.2935485839844</v>
+        <v>332.2935791015625</v>
       </c>
       <c r="G104" t="n">
         <v>22951300</v>
@@ -3041,10 +3041,10 @@
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>326.3532470703125</v>
+        <v>326.3532531738281</v>
       </c>
       <c r="K104" t="n">
-        <v>323.5456115722656</v>
+        <v>323.5456146240234</v>
       </c>
     </row>
     <row r="105">
@@ -3054,16 +3054,16 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>332.3432643804348</v>
+        <v>332.3432341342527</v>
       </c>
       <c r="D105" t="n">
-        <v>337.0152073624945</v>
+        <v>337.0151766911242</v>
       </c>
       <c r="E105" t="n">
-        <v>330.8224029986703</v>
+        <v>330.8223728909</v>
       </c>
       <c r="F105" t="n">
-        <v>335.3253479003906</v>
+        <v>335.3253173828125</v>
       </c>
       <c r="G105" t="n">
         <v>26003800</v>
@@ -3075,7 +3075,7 @@
         <v>0</v>
       </c>
       <c r="J105" t="n">
-        <v>329.1285766601562</v>
+        <v>329.1285705566406</v>
       </c>
       <c r="K105" t="n">
         <v>324.8517654418945</v>
@@ -3088,16 +3088,16 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>335.4645171299162</v>
+        <v>335.4644875433824</v>
       </c>
       <c r="D106" t="n">
-        <v>347.7506863331723</v>
+        <v>347.750655663051</v>
       </c>
       <c r="E106" t="n">
-        <v>335.1861905557903</v>
+        <v>335.1861609938037</v>
       </c>
       <c r="F106" t="n">
-        <v>346.0210876464844</v>
+        <v>346.0210571289062</v>
       </c>
       <c r="G106" t="n">
         <v>38899100</v>
@@ -3109,10 +3109,10 @@
         <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>333.6692932128906</v>
+        <v>333.6692810058594</v>
       </c>
       <c r="K106" t="n">
-        <v>326.5465835571289</v>
+        <v>326.54658203125</v>
       </c>
     </row>
     <row r="107">
@@ -3122,16 +3122,16 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>349.2218529856</v>
+        <v>349.2218216665915</v>
       </c>
       <c r="D107" t="n">
-        <v>349.3709510881127</v>
+        <v>349.3709197557328</v>
       </c>
       <c r="E107" t="n">
-        <v>339.9078173796789</v>
+        <v>339.9077868959742</v>
       </c>
       <c r="F107" t="n">
-        <v>340.2855224609375</v>
+        <v>340.2854919433594</v>
       </c>
       <c r="G107" t="n">
         <v>46533600</v>
@@ -3143,10 +3143,10 @@
         <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>336.7587280273438</v>
+        <v>336.7587097167969</v>
       </c>
       <c r="K107" t="n">
-        <v>327.7299728393555</v>
+        <v>327.7299713134765</v>
       </c>
     </row>
     <row r="108">
@@ -3156,16 +3156,16 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>337.283582191231</v>
+        <v>337.283551559905</v>
       </c>
       <c r="D108" t="n">
-        <v>340.0370283728463</v>
+        <v>340.0369974914586</v>
       </c>
       <c r="E108" t="n">
-        <v>333.8541740271228</v>
+        <v>333.8541437072479</v>
       </c>
       <c r="F108" t="n">
-        <v>336.0310974121094</v>
+        <v>336.0310668945312</v>
       </c>
       <c r="G108" t="n">
         <v>26375400</v>
@@ -3177,10 +3177,10 @@
         <v>0</v>
       </c>
       <c r="J108" t="n">
-        <v>337.9913208007812</v>
+        <v>337.9913024902344</v>
       </c>
       <c r="K108" t="n">
-        <v>328.7095886230469</v>
+        <v>328.709585571289</v>
       </c>
     </row>
     <row r="109">
@@ -3190,16 +3190,16 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>334.3611480019413</v>
+        <v>334.3611172272751</v>
       </c>
       <c r="D109" t="n">
-        <v>335.7130416723274</v>
+        <v>335.7130107732326</v>
       </c>
       <c r="E109" t="n">
-        <v>330.086840317778</v>
+        <v>330.0868099365199</v>
       </c>
       <c r="F109" t="n">
-        <v>331.5679321289062</v>
+        <v>331.5679016113281</v>
       </c>
       <c r="G109" t="n">
         <v>25117800</v>
@@ -3211,10 +3211,10 @@
         <v>0</v>
       </c>
       <c r="J109" t="n">
-        <v>337.8461975097656</v>
+        <v>337.8461669921875</v>
       </c>
       <c r="K109" t="n">
-        <v>329.3248931884766</v>
+        <v>329.3248870849609</v>
       </c>
     </row>
     <row r="110">
@@ -3224,16 +3224,16 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>332.1245409621096</v>
+        <v>332.1245709775148</v>
       </c>
       <c r="D110" t="n">
-        <v>338.0887073541082</v>
+        <v>338.0887379085187</v>
       </c>
       <c r="E110" t="n">
-        <v>331.3492005445626</v>
+        <v>331.3492304898972</v>
       </c>
       <c r="F110" t="n">
-        <v>337.68115234375</v>
+        <v>337.6811828613281</v>
       </c>
       <c r="G110" t="n">
         <v>23556800</v>
@@ -3245,10 +3245,10 @@
         <v>0</v>
       </c>
       <c r="J110" t="n">
-        <v>338.3173583984375</v>
+        <v>338.3173400878906</v>
       </c>
       <c r="K110" t="n">
-        <v>330.5400909423828</v>
+        <v>330.5400848388672</v>
       </c>
     </row>
     <row r="111">
@@ -3279,10 +3279,10 @@
         <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>335.7169799804688</v>
+        <v>335.7169677734375</v>
       </c>
       <c r="K111" t="n">
-        <v>331.5922698974609</v>
+        <v>331.5922637939453</v>
       </c>
     </row>
     <row r="112">
@@ -3313,10 +3313,10 @@
         <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>332.9873840332031</v>
+        <v>332.9873779296875</v>
       </c>
       <c r="K112" t="n">
-        <v>331.7254684448242</v>
+        <v>331.7254638671875</v>
       </c>
     </row>
     <row r="113">
@@ -3326,16 +3326,16 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>329.8780621448217</v>
+        <v>329.8780318744364</v>
       </c>
       <c r="D113" t="n">
-        <v>334.1424500428817</v>
+        <v>334.1424193811861</v>
       </c>
       <c r="E113" t="n">
-        <v>327.3333533188096</v>
+        <v>327.3333232819327</v>
       </c>
       <c r="F113" t="n">
-        <v>332.5718994140625</v>
+        <v>332.5718688964844</v>
       </c>
       <c r="G113" t="n">
         <v>24354100</v>
@@ -3347,10 +3347,10 @@
         <v>0</v>
       </c>
       <c r="J113" t="n">
-        <v>332.2955444335938</v>
+        <v>332.2955383300781</v>
       </c>
       <c r="K113" t="n">
-        <v>331.808967590332</v>
+        <v>331.8089630126953</v>
       </c>
     </row>
     <row r="114">
@@ -3384,7 +3384,7 @@
         <v>332.7508056640625</v>
       </c>
       <c r="K114" t="n">
-        <v>332.0395812988281</v>
+        <v>332.0395767211914</v>
       </c>
     </row>
     <row r="115">
@@ -3415,16 +3415,16 @@
         <v>0</v>
       </c>
       <c r="J115" t="n">
-        <v>331.8243774414062</v>
+        <v>331.8243713378906</v>
       </c>
       <c r="K115" t="n">
-        <v>332.3705917358399</v>
+        <v>332.3705871582031</v>
       </c>
       <c r="M115" t="n">
-        <v>335.7328493437699</v>
+        <v>335.7329098788715</v>
       </c>
       <c r="N115" t="n">
-        <v>34.19760396731175</v>
+        <v>34.19766450241332</v>
       </c>
       <c r="O115" t="n">
         <v>43</v>
@@ -3437,16 +3437,16 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>335.7328493437699</v>
+        <v>335.7329098788715</v>
       </c>
       <c r="D116" t="n">
-        <v>340.6831181171326</v>
+        <v>340.683179544804</v>
       </c>
       <c r="E116" t="n">
-        <v>335.1861462532068</v>
+        <v>335.1862066897338</v>
       </c>
       <c r="F116" t="n">
-        <v>338.5061950683594</v>
+        <v>338.5062561035156</v>
       </c>
       <c r="G116" t="n">
         <v>26823800</v>
@@ -3458,10 +3458,10 @@
         <v>0</v>
       </c>
       <c r="J116" t="n">
-        <v>332.92177734375</v>
+        <v>332.9217834472656</v>
       </c>
       <c r="K116" t="n">
-        <v>332.7662139892578</v>
+        <v>332.7662124633789</v>
       </c>
       <c r="L116" t="n">
         <v>337.1642810024179</v>
@@ -3495,10 +3495,10 @@
         <v>0</v>
       </c>
       <c r="J117" t="n">
-        <v>334.7885559082031</v>
+        <v>334.7885620117187</v>
       </c>
       <c r="K117" t="n">
-        <v>332.8949401855469</v>
+        <v>332.8949371337891</v>
       </c>
     </row>
     <row r="118">
@@ -3529,10 +3529,10 @@
         <v>0</v>
       </c>
       <c r="J118" t="n">
-        <v>335.5002746582031</v>
+        <v>335.5002868652344</v>
       </c>
       <c r="K118" t="n">
-        <v>333.0047790527344</v>
+        <v>333.0047760009766</v>
       </c>
     </row>
     <row r="119">
@@ -3542,16 +3542,16 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>335.28555062847</v>
+        <v>335.2855204659035</v>
       </c>
       <c r="D119" t="n">
-        <v>340.9415709981333</v>
+        <v>340.9415403267466</v>
       </c>
       <c r="E119" t="n">
-        <v>333.4963127982555</v>
+        <v>333.4962827966504</v>
       </c>
       <c r="F119" t="n">
-        <v>339.2318420410156</v>
+        <v>339.2318115234375</v>
       </c>
       <c r="G119" t="n">
         <v>28161200</v>
@@ -3563,10 +3563,10 @@
         <v>0</v>
       </c>
       <c r="J119" t="n">
-        <v>336.5777954101562</v>
+        <v>336.5778015136719</v>
       </c>
       <c r="K119" t="n">
-        <v>333.3820114135742</v>
+        <v>333.3820068359375</v>
       </c>
     </row>
     <row r="120">
@@ -3576,16 +3576,16 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>337.2935191268303</v>
+        <v>337.2934884192068</v>
       </c>
       <c r="D120" t="n">
-        <v>339.7487689971467</v>
+        <v>339.7487380659941</v>
       </c>
       <c r="E120" t="n">
-        <v>334.9873673588974</v>
+        <v>334.9873368612288</v>
       </c>
       <c r="F120" t="n">
-        <v>335.2060546875</v>
+        <v>335.2060241699219</v>
       </c>
       <c r="G120" t="n">
         <v>21185300</v>
@@ -3600,7 +3600,7 @@
         <v>337.0092041015625</v>
       </c>
       <c r="K120" t="n">
-        <v>334.0698791503906</v>
+        <v>334.0698715209961</v>
       </c>
     </row>
     <row r="121">
@@ -3610,16 +3610,16 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>332.6016817703048</v>
+        <v>332.6017125426347</v>
       </c>
       <c r="D121" t="n">
-        <v>333.227924088669</v>
+        <v>333.2279549189389</v>
       </c>
       <c r="E121" t="n">
-        <v>325.6335377334161</v>
+        <v>325.6335678610529</v>
       </c>
       <c r="F121" t="n">
-        <v>329.8482055664062</v>
+        <v>329.8482360839844</v>
       </c>
       <c r="G121" t="n">
         <v>32791400</v>
@@ -3631,10 +3631,10 @@
         <v>0</v>
       </c>
       <c r="J121" t="n">
-        <v>335.2776062011719</v>
+        <v>335.2776000976563</v>
       </c>
       <c r="K121" t="n">
-        <v>334.3964141845703</v>
+        <v>334.3964080810547</v>
       </c>
     </row>
     <row r="122">
@@ -3665,16 +3665,16 @@
         <v>0</v>
       </c>
       <c r="J122" t="n">
-        <v>334.1802001953125</v>
+        <v>334.1801940917969</v>
       </c>
       <c r="K122" t="n">
-        <v>334.6787170410156</v>
+        <v>334.6787109375</v>
       </c>
       <c r="M122" t="n">
-        <v>334.5897649944963</v>
+        <v>334.5897954577721</v>
       </c>
       <c r="N122" t="n">
-        <v>-2.574516007921602</v>
+        <v>-2.574485544645768</v>
       </c>
       <c r="O122" t="n">
         <v>6</v>
@@ -3687,16 +3687,16 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>334.5897649944963</v>
+        <v>334.5897954577721</v>
       </c>
       <c r="D123" t="n">
-        <v>339.6095932720836</v>
+        <v>339.609624192398</v>
       </c>
       <c r="E123" t="n">
-        <v>333.6653264169743</v>
+        <v>333.665356796083</v>
       </c>
       <c r="F123" t="n">
-        <v>335.1861877441406</v>
+        <v>335.1862182617188</v>
       </c>
       <c r="G123" t="n">
         <v>29995300</v>
@@ -3711,7 +3711,7 @@
         <v>333.9913391113281</v>
       </c>
       <c r="K123" t="n">
-        <v>334.9446197509766</v>
+        <v>334.9446166992187</v>
       </c>
     </row>
     <row r="124">
@@ -3742,10 +3742,10 @@
         <v>0</v>
       </c>
       <c r="J124" t="n">
-        <v>334.2676818847656</v>
+        <v>334.2676879882812</v>
       </c>
       <c r="K124" t="n">
-        <v>335.3606201171875</v>
+        <v>335.3606155395508</v>
       </c>
     </row>
     <row r="125">
@@ -3776,10 +3776,10 @@
         <v>0</v>
       </c>
       <c r="J125" t="n">
-        <v>335.8620971679687</v>
+        <v>335.862109375</v>
       </c>
       <c r="K125" t="n">
-        <v>335.7532592773438</v>
+        <v>335.7532562255859</v>
       </c>
       <c r="L125" t="n">
         <v>343.6155330928394</v>
@@ -3813,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>338.6255065917969</v>
+        <v>338.6255126953125</v>
       </c>
       <c r="K126" t="n">
-        <v>335.6354675292969</v>
+        <v>335.6354660034179</v>
       </c>
     </row>
     <row r="127">
@@ -3826,16 +3826,16 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>343.7646539141556</v>
+        <v>343.7645951982308</v>
       </c>
       <c r="D127" t="n">
-        <v>364.5895504687594</v>
+        <v>364.5894881958863</v>
       </c>
       <c r="E127" t="n">
-        <v>340.1265385100075</v>
+        <v>340.1264804154825</v>
       </c>
       <c r="F127" t="n">
-        <v>357.3430786132812</v>
+        <v>357.343017578125</v>
       </c>
       <c r="G127" t="n">
         <v>64872700</v>
@@ -3847,10 +3847,10 @@
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>343.9972412109375</v>
+        <v>343.9972351074219</v>
       </c>
       <c r="K127" t="n">
-        <v>336.4883453369141</v>
+        <v>336.4883422851562</v>
       </c>
     </row>
     <row r="128">
@@ -3860,16 +3860,16 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>359.5895599376757</v>
+        <v>359.5895288468389</v>
       </c>
       <c r="D128" t="n">
-        <v>360.2953111882384</v>
+        <v>360.295280036381</v>
       </c>
       <c r="E128" t="n">
-        <v>350.3351634618897</v>
+        <v>350.3351331712067</v>
       </c>
       <c r="F128" t="n">
-        <v>352.9593811035156</v>
+        <v>352.9593505859375</v>
       </c>
       <c r="G128" t="n">
         <v>39732900</v>
@@ -3881,10 +3881,10 @@
         <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>347.5518798828125</v>
+        <v>347.5518615722656</v>
       </c>
       <c r="K128" t="n">
-        <v>337.3347595214844</v>
+        <v>337.3347564697266</v>
       </c>
     </row>
     <row r="129">
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>348.3888488769531</v>
+        <v>348.3888305664062</v>
       </c>
       <c r="K129" t="n">
-        <v>337.9962829589844</v>
+        <v>337.9962814331055</v>
       </c>
     </row>
     <row r="130">
@@ -3949,10 +3949,10 @@
         <v>0</v>
       </c>
       <c r="J130" t="n">
-        <v>348.0966064453125</v>
+        <v>348.0965881347656</v>
       </c>
       <c r="K130" t="n">
-        <v>338.1980712890625</v>
+        <v>338.1980682373047</v>
       </c>
     </row>
     <row r="131">
@@ -3983,10 +3983,10 @@
         <v>0</v>
       </c>
       <c r="J131" t="n">
-        <v>347.97333984375</v>
+        <v>347.9733215332031</v>
       </c>
       <c r="K131" t="n">
-        <v>338.6995574951172</v>
+        <v>338.6995544433594</v>
       </c>
     </row>
     <row r="132">
@@ -3996,16 +3996,16 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>345.036937449727</v>
+        <v>345.0369676308079</v>
       </c>
       <c r="D132" t="n">
-        <v>349.7884189371964</v>
+        <v>349.788449533899</v>
       </c>
       <c r="E132" t="n">
-        <v>343.0091428004128</v>
+        <v>343.0091728041184</v>
       </c>
       <c r="F132" t="n">
-        <v>348.8838500976562</v>
+        <v>348.8838806152344</v>
       </c>
       <c r="G132" t="n">
         <v>41637700</v>
@@ -4020,7 +4020,7 @@
         <v>346.281494140625</v>
       </c>
       <c r="K132" t="n">
-        <v>339.8118728637695</v>
+        <v>339.8118713378906</v>
       </c>
     </row>
     <row r="133">
@@ -4051,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="J133" t="n">
-        <v>342.8401672363281</v>
+        <v>342.8401733398438</v>
       </c>
       <c r="K133" t="n">
         <v>339.9709152221679</v>
@@ -4085,16 +4085,16 @@
         <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>339.6294616699219</v>
+        <v>339.6294677734375</v>
       </c>
       <c r="K134" t="n">
         <v>339.7159469604492</v>
       </c>
       <c r="M134" t="n">
-        <v>331.6772395722927</v>
+        <v>331.6772696659797</v>
       </c>
       <c r="N134" t="n">
-        <v>-11.93829352054667</v>
+        <v>-11.93826342685969</v>
       </c>
       <c r="O134" t="n">
         <v>9</v>
@@ -4107,16 +4107,16 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>331.6772395722927</v>
+        <v>331.6772696659797</v>
       </c>
       <c r="D135" t="n">
-        <v>337.9793716178067</v>
+        <v>337.9794022832977</v>
       </c>
       <c r="E135" t="n">
-        <v>331.1802257169495</v>
+        <v>331.1802557655415</v>
       </c>
       <c r="F135" t="n">
-        <v>336.3491516113281</v>
+        <v>336.3491821289062</v>
       </c>
       <c r="G135" t="n">
         <v>28484900</v>
@@ -4128,10 +4128,10 @@
         <v>0</v>
       </c>
       <c r="J135" t="n">
-        <v>338.555908203125</v>
+        <v>338.5559204101563</v>
       </c>
       <c r="K135" t="n">
-        <v>339.8809539794922</v>
+        <v>339.8809555053711</v>
       </c>
     </row>
     <row r="136">
@@ -4162,10 +4162,10 @@
         <v>0</v>
       </c>
       <c r="J136" t="n">
-        <v>336.7288879394531</v>
+        <v>336.7289001464844</v>
       </c>
       <c r="K136" t="n">
-        <v>339.6513351440429</v>
+        <v>339.6513336181641</v>
       </c>
     </row>
     <row r="137">
@@ -4196,10 +4196,10 @@
         <v>0</v>
       </c>
       <c r="J137" t="n">
-        <v>333.8183776855469</v>
+        <v>333.8183837890625</v>
       </c>
       <c r="K137" t="n">
-        <v>339.5693283081055</v>
+        <v>339.5693267822265</v>
       </c>
     </row>
     <row r="138">
@@ -4230,10 +4230,10 @@
         <v>0</v>
       </c>
       <c r="J138" t="n">
-        <v>331.7766479492187</v>
+        <v>331.7766540527344</v>
       </c>
       <c r="K138" t="n">
-        <v>339.0400085449219</v>
+        <v>339.0400070190429</v>
       </c>
     </row>
     <row r="139">
@@ -4243,16 +4243,16 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>324.0530749500537</v>
+        <v>324.0530444941351</v>
       </c>
       <c r="D139" t="n">
-        <v>327.9099078123132</v>
+        <v>327.9098769939127</v>
       </c>
       <c r="E139" t="n">
-        <v>324.0033856923191</v>
+        <v>324.0033552410705</v>
       </c>
       <c r="F139" t="n">
-        <v>324.7091369628906</v>
+        <v>324.7091064453125</v>
       </c>
       <c r="G139" t="n">
         <v>18253700</v>
@@ -4267,7 +4267,7 @@
         <v>330.9695007324219</v>
       </c>
       <c r="K139" t="n">
-        <v>338.3138732910156</v>
+        <v>338.3138717651367</v>
       </c>
     </row>
     <row r="140">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="J140" t="n">
-        <v>328.8641540527344</v>
+        <v>328.8641479492188</v>
       </c>
       <c r="K140" t="n">
         <v>337.8446914672851</v>
@@ -4332,10 +4332,10 @@
         <v>0</v>
       </c>
       <c r="J141" t="n">
-        <v>327.7090942382812</v>
+        <v>327.7090881347656</v>
       </c>
       <c r="K141" t="n">
-        <v>337.7592071533203</v>
+        <v>337.7592056274414</v>
       </c>
     </row>
     <row r="142">
@@ -4366,10 +4366,10 @@
         <v>0</v>
       </c>
       <c r="J142" t="n">
-        <v>325.6633850097656</v>
+        <v>325.66337890625</v>
       </c>
       <c r="K142" t="n">
-        <v>337.4401245117188</v>
+        <v>337.4401229858398</v>
       </c>
     </row>
     <row r="143">
@@ -4379,16 +4379,16 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>324.5202713777388</v>
+        <v>324.5202404586021</v>
       </c>
       <c r="D143" t="n">
-        <v>325.1564334234011</v>
+        <v>325.1564024436531</v>
       </c>
       <c r="E143" t="n">
-        <v>319.1326271168186</v>
+        <v>319.1325967109974</v>
       </c>
       <c r="F143" t="n">
-        <v>320.3056030273438</v>
+        <v>320.3055725097656</v>
       </c>
       <c r="G143" t="n">
         <v>22373300</v>
@@ -4400,10 +4400,10 @@
         <v>0</v>
       </c>
       <c r="J143" t="n">
-        <v>324.6156860351563</v>
+        <v>324.615673828125</v>
       </c>
       <c r="K143" t="n">
-        <v>336.6960952758789</v>
+        <v>336.6960906982422</v>
       </c>
     </row>
     <row r="144">
@@ -4413,16 +4413,16 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>324.0729153912347</v>
+        <v>324.0729462008241</v>
       </c>
       <c r="D144" t="n">
-        <v>326.2995581741466</v>
+        <v>326.2995891954228</v>
       </c>
       <c r="E144" t="n">
-        <v>319.2618247325042</v>
+        <v>319.2618550847035</v>
       </c>
       <c r="F144" t="n">
-        <v>321.0013732910156</v>
+        <v>321.0014038085938</v>
       </c>
       <c r="G144" t="n">
         <v>20113700</v>
@@ -4437,7 +4437,7 @@
         <v>323.8741333007812</v>
       </c>
       <c r="K144" t="n">
-        <v>335.7154861450196</v>
+        <v>335.7154830932617</v>
       </c>
     </row>
     <row r="145">
@@ -4471,7 +4471,7 @@
         <v>322.52822265625</v>
       </c>
       <c r="K145" t="n">
-        <v>334.5112228393555</v>
+        <v>334.5112197875977</v>
       </c>
     </row>
     <row r="146">
@@ -4481,16 +4481,16 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>319.4705690562157</v>
+        <v>319.4706295922275</v>
       </c>
       <c r="D146" t="n">
-        <v>322.1246059609124</v>
+        <v>322.1246669998338</v>
       </c>
       <c r="E146" t="n">
-        <v>318.1683648933637</v>
+        <v>318.1684251826227</v>
       </c>
       <c r="F146" t="n">
-        <v>322.104736328125</v>
+        <v>322.1047973632812</v>
       </c>
       <c r="G146" t="n">
         <v>18836100</v>
@@ -4502,7 +4502,7 @@
         <v>0</v>
       </c>
       <c r="J146" t="n">
-        <v>321.3214660644531</v>
+        <v>321.3214782714844</v>
       </c>
       <c r="K146" t="n">
         <v>333.4331970214844</v>
@@ -4536,10 +4536,10 @@
         <v>0</v>
       </c>
       <c r="J147" t="n">
-        <v>320.4884704589844</v>
+        <v>320.4884826660156</v>
       </c>
       <c r="K147" t="n">
-        <v>331.5629318237305</v>
+        <v>331.5629348754883</v>
       </c>
     </row>
     <row r="148">
@@ -4570,10 +4570,10 @@
         <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>320.2595092773437</v>
+        <v>320.2595275878906</v>
       </c>
       <c r="K148" t="n">
-        <v>329.8730026245117</v>
+        <v>329.8730072021484</v>
       </c>
     </row>
     <row r="149">
@@ -4604,10 +4604,10 @@
         <v>0</v>
       </c>
       <c r="J149" t="n">
-        <v>319.1901245117188</v>
+        <v>319.19013671875</v>
       </c>
       <c r="K149" t="n">
-        <v>328.4158050537109</v>
+        <v>328.4158096313477</v>
       </c>
     </row>
     <row r="150">
@@ -4638,10 +4638,10 @@
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>318.4227478027344</v>
+        <v>318.4227600097656</v>
       </c>
       <c r="K150" t="n">
-        <v>327.0927581787109</v>
+        <v>327.0927627563477</v>
       </c>
     </row>
     <row r="151">
@@ -4651,16 +4651,16 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>316.7003661841551</v>
+        <v>316.7003360410794</v>
       </c>
       <c r="D151" t="n">
-        <v>321.5216433453291</v>
+        <v>321.5216127433712</v>
       </c>
       <c r="E151" t="n">
-        <v>315.8138241571855</v>
+        <v>315.8137940984894</v>
       </c>
       <c r="F151" t="n">
-        <v>320.6351013183594</v>
+        <v>320.6350708007812</v>
       </c>
       <c r="G151" t="n">
         <v>24040000</v>
@@ -4672,10 +4672,10 @@
         <v>0</v>
       </c>
       <c r="J151" t="n">
-        <v>318.1288208007812</v>
+        <v>318.1288146972656</v>
       </c>
       <c r="K151" t="n">
-        <v>325.9720672607422</v>
+        <v>325.9720703125</v>
       </c>
     </row>
     <row r="152">
@@ -4706,10 +4706,10 @@
         <v>0</v>
       </c>
       <c r="J152" t="n">
-        <v>318.3838317871094</v>
+        <v>318.3838256835937</v>
       </c>
       <c r="K152" t="n">
-        <v>324.5885162353516</v>
+        <v>324.5885177612305</v>
       </c>
     </row>
     <row r="153">
@@ -4740,10 +4740,10 @@
         <v>0</v>
       </c>
       <c r="J153" t="n">
-        <v>319.69873046875</v>
+        <v>319.6987243652344</v>
       </c>
       <c r="K153" t="n">
-        <v>324.0876434326172</v>
+        <v>324.0876449584961</v>
       </c>
     </row>
     <row r="154">
@@ -4774,10 +4774,10 @@
         <v>0</v>
       </c>
       <c r="J154" t="n">
-        <v>320.3143371582031</v>
+        <v>320.3143310546875</v>
       </c>
       <c r="K154" t="n">
-        <v>323.5870239257812</v>
+        <v>323.5870254516602</v>
       </c>
     </row>
     <row r="155">
@@ -4808,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="J155" t="n">
-        <v>321.6093078613281</v>
+        <v>321.6093017578125</v>
       </c>
       <c r="K155" t="n">
         <v>322.8561080932617</v>
@@ -4882,7 +4882,7 @@
         <v>321.9232467651367</v>
       </c>
       <c r="L157" t="n">
-        <v>327.3988405611436</v>
+        <v>327.3988100547031</v>
       </c>
     </row>
     <row r="158">
@@ -4892,16 +4892,16 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>327.3988405611436</v>
+        <v>327.3988100547031</v>
       </c>
       <c r="D158" t="n">
-        <v>328.5344156591241</v>
+        <v>328.5343850468728</v>
       </c>
       <c r="E158" t="n">
-        <v>325.1874254760788</v>
+        <v>325.1873951756941</v>
       </c>
       <c r="F158" t="n">
-        <v>327.5183715820312</v>
+        <v>327.5183410644531</v>
       </c>
       <c r="G158" t="n">
         <v>15222100</v>
@@ -4913,10 +4913,10 @@
         <v>0</v>
       </c>
       <c r="J158" t="n">
-        <v>323.513916015625</v>
+        <v>323.5139099121094</v>
       </c>
       <c r="K158" t="n">
-        <v>322.0219604492187</v>
+        <v>322.0219589233399</v>
       </c>
     </row>
     <row r="159">
@@ -4947,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="J159" t="n">
-        <v>325.0658935546875</v>
+        <v>325.0658874511719</v>
       </c>
       <c r="K159" t="n">
         <v>322.1111221313477</v>
@@ -4981,7 +4981,7 @@
         <v>0</v>
       </c>
       <c r="J160" t="n">
-        <v>326.1974975585937</v>
+        <v>326.1974914550781</v>
       </c>
       <c r="K160" t="n">
         <v>322.1894439697265</v>
@@ -5015,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="J161" t="n">
-        <v>328.1598693847656</v>
+        <v>328.15986328125</v>
       </c>
       <c r="K161" t="n">
         <v>322.3955139160156</v>
@@ -5049,7 +5049,7 @@
         <v>0</v>
       </c>
       <c r="J162" t="n">
-        <v>329.0504150390625</v>
+        <v>329.0504089355469</v>
       </c>
       <c r="K162" t="n">
         <v>322.7700042724609</v>
@@ -5086,7 +5086,7 @@
         <v>329.2735473632812</v>
       </c>
       <c r="K163" t="n">
-        <v>323.18642578125</v>
+        <v>323.1864273071289</v>
       </c>
     </row>
     <row r="164">
@@ -5188,7 +5188,7 @@
         <v>332.0647033691406</v>
       </c>
       <c r="K166" t="n">
-        <v>325.0813232421875</v>
+        <v>325.0813201904297</v>
       </c>
     </row>
     <row r="167">
@@ -5222,7 +5222,7 @@
         <v>332.6982421875</v>
       </c>
       <c r="K167" t="n">
-        <v>325.8224472045898</v>
+        <v>325.822444152832</v>
       </c>
     </row>
     <row r="168">
@@ -5232,16 +5232,16 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>337.8382559337177</v>
+        <v>337.8382864918402</v>
       </c>
       <c r="D168" t="n">
-        <v>339.5416336168719</v>
+        <v>339.5416643290682</v>
       </c>
       <c r="E168" t="n">
-        <v>335.2682480328104</v>
+        <v>335.2682783584707</v>
       </c>
       <c r="F168" t="n">
-        <v>337.3900146484375</v>
+        <v>337.3900451660156</v>
       </c>
       <c r="G168" t="n">
         <v>20267000</v>
@@ -5253,10 +5253,10 @@
         <v>0</v>
       </c>
       <c r="J168" t="n">
-        <v>334.4494384765625</v>
+        <v>334.4494445800781</v>
       </c>
       <c r="K168" t="n">
-        <v>326.7339080810547</v>
+        <v>326.7339065551758</v>
       </c>
     </row>
     <row r="169">
@@ -5266,16 +5266,16 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>335.6169086433574</v>
+        <v>335.6169397801232</v>
       </c>
       <c r="D169" t="n">
-        <v>336.0950326927191</v>
+        <v>336.0950638738427</v>
       </c>
       <c r="E169" t="n">
-        <v>328.3750073504314</v>
+        <v>328.3750378153318</v>
       </c>
       <c r="F169" t="n">
-        <v>328.9428100585938</v>
+        <v>328.9428405761719</v>
       </c>
       <c r="G169" t="n">
         <v>37666900</v>
@@ -5287,7 +5287,7 @@
         <v>0</v>
       </c>
       <c r="J169" t="n">
-        <v>333.6425720214844</v>
+        <v>333.6425842285156</v>
       </c>
       <c r="K169" t="n">
         <v>327.3983261108398</v>
@@ -5300,16 +5300,16 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>326.5321560535634</v>
+        <v>326.5321864542861</v>
       </c>
       <c r="D170" t="n">
-        <v>329.1221061156409</v>
+        <v>329.1221367574925</v>
       </c>
       <c r="E170" t="n">
-        <v>325.0977231083988</v>
+        <v>325.0977533755733</v>
       </c>
       <c r="F170" t="n">
-        <v>327.7872924804688</v>
+        <v>327.7873229980469</v>
       </c>
       <c r="G170" t="n">
         <v>16834200</v>
@@ -5321,10 +5321,10 @@
         <v>0</v>
       </c>
       <c r="J170" t="n">
-        <v>331.8734375</v>
+        <v>331.8734558105469</v>
       </c>
       <c r="K170" t="n">
-        <v>328.0248916625977</v>
+        <v>328.0248931884765</v>
       </c>
     </row>
     <row r="171">
@@ -5334,16 +5334,16 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>324.9084870734358</v>
+        <v>324.9085173607294</v>
       </c>
       <c r="D171" t="n">
-        <v>328.1160343093041</v>
+        <v>328.1160648955986</v>
       </c>
       <c r="E171" t="n">
-        <v>323.2549038003314</v>
+        <v>323.2549339334814</v>
       </c>
       <c r="F171" t="n">
-        <v>327.3788757324219</v>
+        <v>327.37890625</v>
       </c>
       <c r="G171" t="n">
         <v>16505900</v>
@@ -5355,10 +5355,10 @@
         <v>0</v>
       </c>
       <c r="J171" t="n">
-        <v>331.2518493652344</v>
+        <v>331.2518737792969</v>
       </c>
       <c r="K171" t="n">
-        <v>328.3620803833008</v>
+        <v>328.3620849609375</v>
       </c>
     </row>
     <row r="172">
@@ -5368,16 +5368,16 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>328.2356065321914</v>
+        <v>328.2355751831007</v>
       </c>
       <c r="D172" t="n">
-        <v>328.3152837507399</v>
+        <v>328.3152523940395</v>
       </c>
       <c r="E172" t="n">
-        <v>319.2704146677896</v>
+        <v>319.2703841749455</v>
       </c>
       <c r="F172" t="n">
-        <v>319.5293884277344</v>
+        <v>319.5293579101562</v>
       </c>
       <c r="G172" t="n">
         <v>21436500</v>
@@ -5389,16 +5389,16 @@
         <v>0</v>
       </c>
       <c r="J172" t="n">
-        <v>328.2056762695312</v>
+        <v>328.2056945800781</v>
       </c>
       <c r="K172" t="n">
-        <v>328.2779083251953</v>
+        <v>328.2779113769531</v>
       </c>
       <c r="M172" t="n">
-        <v>318.0252446448246</v>
+        <v>318.0252141530325</v>
       </c>
       <c r="N172" t="n">
-        <v>-9.373595916319005</v>
+        <v>-9.373595901670626</v>
       </c>
       <c r="O172" t="n">
         <v>15</v>
@@ -5411,16 +5411,16 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>318.0252446448246</v>
+        <v>318.0252141530325</v>
       </c>
       <c r="D173" t="n">
-        <v>324.0916874062139</v>
+        <v>324.0916563327802</v>
       </c>
       <c r="E173" t="n">
-        <v>313.7817108276803</v>
+        <v>313.781680742752</v>
       </c>
       <c r="F173" t="n">
-        <v>318.294189453125</v>
+        <v>318.2941589355469</v>
       </c>
       <c r="G173" t="n">
         <v>35529500</v>
@@ -5432,10 +5432,10 @@
         <v>0</v>
       </c>
       <c r="J173" t="n">
-        <v>324.3865112304687</v>
+        <v>324.3865173339844</v>
       </c>
       <c r="K173" t="n">
-        <v>327.9058532714844</v>
+        <v>327.9058547973633</v>
       </c>
     </row>
     <row r="174">
@@ -5469,7 +5469,7 @@
         <v>321.754736328125</v>
       </c>
       <c r="K174" t="n">
-        <v>327.7584259033203</v>
+        <v>327.7584274291992</v>
       </c>
     </row>
     <row r="175">
@@ -5500,10 +5500,10 @@
         <v>0</v>
       </c>
       <c r="J175" t="n">
-        <v>319.4596557617188</v>
+        <v>319.4596496582031</v>
       </c>
       <c r="K175" t="n">
-        <v>327.4874786376953</v>
+        <v>327.4874801635742</v>
       </c>
     </row>
     <row r="176">
@@ -5534,10 +5534,10 @@
         <v>0</v>
       </c>
       <c r="J176" t="n">
-        <v>316.1704345703125</v>
+        <v>316.1704223632813</v>
       </c>
       <c r="K176" t="n">
-        <v>326.9117141723633</v>
+        <v>326.9117156982422</v>
       </c>
     </row>
     <row r="177">
@@ -5568,10 +5568,10 @@
         <v>0</v>
       </c>
       <c r="J177" t="n">
-        <v>314.5806030273437</v>
+        <v>314.5805969238281</v>
       </c>
       <c r="K177" t="n">
-        <v>326.1337341308594</v>
+        <v>326.1337356567383</v>
       </c>
     </row>
     <row r="178">
@@ -5605,7 +5605,7 @@
         <v>313.4071594238281</v>
       </c>
       <c r="K178" t="n">
-        <v>325.3791641235351</v>
+        <v>325.379167175293</v>
       </c>
     </row>
     <row r="179">
@@ -5615,16 +5615,16 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>316.521073414613</v>
+        <v>316.5210427037327</v>
       </c>
       <c r="D179" t="n">
-        <v>318.2344223765372</v>
+        <v>318.2343914994169</v>
       </c>
       <c r="E179" t="n">
-        <v>313.7617975815552</v>
+        <v>313.7617671383974</v>
       </c>
       <c r="F179" t="n">
-        <v>314.52880859375</v>
+        <v>314.5287780761719</v>
       </c>
       <c r="G179" t="n">
         <v>24140300</v>
@@ -5636,10 +5636,10 @@
         <v>0</v>
       </c>
       <c r="J179" t="n">
-        <v>313.1561340332031</v>
+        <v>313.1561279296875</v>
       </c>
       <c r="K179" t="n">
-        <v>324.7809860229492</v>
+        <v>324.7809875488281</v>
       </c>
     </row>
     <row r="180">
@@ -5670,10 +5670,10 @@
         <v>0</v>
       </c>
       <c r="J180" t="n">
-        <v>314.004833984375</v>
+        <v>314.0048278808594</v>
       </c>
       <c r="K180" t="n">
-        <v>324.4393127441406</v>
+        <v>324.4393142700195</v>
       </c>
     </row>
     <row r="181">
@@ -5683,16 +5683,16 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>319.5891138579261</v>
+        <v>319.5891451000006</v>
       </c>
       <c r="D181" t="n">
-        <v>320.1469759159947</v>
+        <v>320.1470072126041</v>
       </c>
       <c r="E181" t="n">
-        <v>310.0063259531334</v>
+        <v>310.0063562584232</v>
       </c>
       <c r="F181" t="n">
-        <v>312.1779174804688</v>
+        <v>312.1779479980469</v>
       </c>
       <c r="G181" t="n">
         <v>21033500</v>
@@ -5707,7 +5707,7 @@
         <v>314.2538635253906</v>
       </c>
       <c r="K181" t="n">
-        <v>323.4352127075196</v>
+        <v>323.4352157592774</v>
       </c>
     </row>
     <row r="182">
@@ -5741,7 +5741,7 @@
         <v>315.4830932617188</v>
       </c>
       <c r="K182" t="n">
-        <v>322.7419036865234</v>
+        <v>322.7419067382813</v>
       </c>
     </row>
     <row r="183">
@@ -5775,7 +5775,7 @@
         <v>316.6226623535156</v>
       </c>
       <c r="K183" t="n">
-        <v>322.2164428710938</v>
+        <v>322.2164459228516</v>
       </c>
     </row>
     <row r="184">
@@ -5806,10 +5806,10 @@
         <v>0</v>
       </c>
       <c r="J184" t="n">
-        <v>318.9157592773437</v>
+        <v>318.9157653808594</v>
       </c>
       <c r="K184" t="n">
-        <v>321.867300415039</v>
+        <v>321.8673034667969</v>
       </c>
     </row>
     <row r="185">
@@ -5840,10 +5840,10 @@
         <v>0</v>
       </c>
       <c r="J185" t="n">
-        <v>320.5135559082031</v>
+        <v>320.5135620117188</v>
       </c>
       <c r="K185" t="n">
-        <v>321.4628707885742</v>
+        <v>321.462873840332</v>
       </c>
     </row>
     <row r="186">
@@ -5877,7 +5877,7 @@
         <v>323.5019592285156</v>
       </c>
       <c r="K186" t="n">
-        <v>321.2945266723633</v>
+        <v>321.2945297241211</v>
       </c>
       <c r="L186" t="n">
         <v>329.9289963141856</v>
@@ -5914,7 +5914,7 @@
         <v>326.1835510253906</v>
       </c>
       <c r="K187" t="n">
-        <v>321.1132308959961</v>
+        <v>321.1132339477539</v>
       </c>
     </row>
     <row r="188">
@@ -5924,16 +5924,16 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>329.2914969538185</v>
+        <v>329.2914664906106</v>
       </c>
       <c r="D188" t="n">
-        <v>332.3396596861262</v>
+        <v>332.3396289409286</v>
       </c>
       <c r="E188" t="n">
-        <v>327.4486459216531</v>
+        <v>327.4486156289299</v>
       </c>
       <c r="F188" t="n">
-        <v>329.8792114257812</v>
+        <v>329.8791809082031</v>
       </c>
       <c r="G188" t="n">
         <v>19313100</v>
@@ -5945,7 +5945,7 @@
         <v>0</v>
       </c>
       <c r="J188" t="n">
-        <v>328.5344299316406</v>
+        <v>328.534423828125</v>
       </c>
       <c r="K188" t="n">
         <v>320.7376907348633</v>
@@ -5958,16 +5958,16 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>331.0945036397515</v>
+        <v>331.0944726891751</v>
       </c>
       <c r="D189" t="n">
-        <v>332.538877430905</v>
+        <v>332.5388463453091</v>
       </c>
       <c r="E189" t="n">
-        <v>325.097766924787</v>
+        <v>325.0977365347831</v>
       </c>
       <c r="F189" t="n">
-        <v>326.4624938964844</v>
+        <v>326.4624633789062</v>
       </c>
       <c r="G189" t="n">
         <v>21072400</v>
@@ -5979,10 +5979,10 @@
         <v>0</v>
       </c>
       <c r="J189" t="n">
-        <v>328.6280700683594</v>
+        <v>328.6280578613281</v>
       </c>
       <c r="K189" t="n">
-        <v>320.6136749267578</v>
+        <v>320.613671875</v>
       </c>
     </row>
     <row r="190">
@@ -5992,16 +5992,16 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>329.7696078924969</v>
+        <v>329.7695775207935</v>
       </c>
       <c r="D190" t="n">
-        <v>334.8399483914669</v>
+        <v>334.8399175527863</v>
       </c>
       <c r="E190" t="n">
-        <v>329.3213665671338</v>
+        <v>329.3213362367134</v>
       </c>
       <c r="F190" t="n">
-        <v>331.3534851074219</v>
+        <v>331.3534545898438</v>
       </c>
       <c r="G190" t="n">
         <v>22158000</v>
@@ -6013,10 +6013,10 @@
         <v>0</v>
       </c>
       <c r="J190" t="n">
-        <v>329.189892578125</v>
+        <v>329.1898742675781</v>
       </c>
       <c r="K190" t="n">
-        <v>320.7919845581055</v>
+        <v>320.7919784545899</v>
       </c>
     </row>
     <row r="191">
@@ -6026,16 +6026,16 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>328.3152477540011</v>
+        <v>328.3152780445767</v>
       </c>
       <c r="D191" t="n">
-        <v>332.1702749690978</v>
+        <v>332.1703056153407</v>
       </c>
       <c r="E191" t="n">
-        <v>326.1436865919406</v>
+        <v>326.1437166821666</v>
       </c>
       <c r="F191" t="n">
-        <v>330.7756958007812</v>
+        <v>330.7757263183594</v>
       </c>
       <c r="G191" t="n">
         <v>18338500</v>
@@ -6047,10 +6047,10 @@
         <v>0</v>
       </c>
       <c r="J191" t="n">
-        <v>329.921044921875</v>
+        <v>329.9210327148438</v>
       </c>
       <c r="K191" t="n">
-        <v>320.9618255615234</v>
+        <v>320.9618194580078</v>
       </c>
     </row>
     <row r="192">
@@ -6081,10 +6081,10 @@
         <v>0</v>
       </c>
       <c r="J192" t="n">
-        <v>329.4608276367188</v>
+        <v>329.4608154296875</v>
       </c>
       <c r="K192" t="n">
-        <v>321.427018737793</v>
+        <v>321.4270141601563</v>
       </c>
     </row>
     <row r="193">
@@ -6115,10 +6115,10 @@
         <v>0</v>
       </c>
       <c r="J193" t="n">
-        <v>329.4927001953125</v>
+        <v>329.4926940917969</v>
       </c>
       <c r="K193" t="n">
-        <v>322.0142379760742</v>
+        <v>322.0142349243164</v>
       </c>
     </row>
     <row r="194">
@@ -6152,7 +6152,7 @@
         <v>329.2815185546875</v>
       </c>
       <c r="K194" t="n">
-        <v>322.4953704833985</v>
+        <v>322.4953674316406</v>
       </c>
     </row>
     <row r="195">
@@ -6162,16 +6162,16 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>324.2112099055406</v>
+        <v>324.2111797447366</v>
       </c>
       <c r="D195" t="n">
-        <v>331.4431407784667</v>
+        <v>331.4431099448888</v>
       </c>
       <c r="E195" t="n">
-        <v>323.1354003010832</v>
+        <v>323.1353702403599</v>
       </c>
       <c r="F195" t="n">
-        <v>328.0463256835938</v>
+        <v>328.0462951660156</v>
       </c>
       <c r="G195" t="n">
         <v>24374700</v>
@@ -6186,7 +6186,7 @@
         <v>328.6200866699219</v>
       </c>
       <c r="K195" t="n">
-        <v>323.0820922851562</v>
+        <v>323.0820877075195</v>
       </c>
     </row>
     <row r="196">
@@ -6196,16 +6196,16 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>330.0186589696724</v>
+        <v>330.0186283810018</v>
       </c>
       <c r="D196" t="n">
-        <v>330.5565789889712</v>
+        <v>330.556548350442</v>
       </c>
       <c r="E196" t="n">
-        <v>326.3329872511189</v>
+        <v>326.3329570040647</v>
       </c>
       <c r="F196" t="n">
-        <v>329.2516479492188</v>
+        <v>329.2516174316406</v>
       </c>
       <c r="G196" t="n">
         <v>31153600</v>
@@ -6217,10 +6217,10 @@
         <v>0</v>
       </c>
       <c r="J196" t="n">
-        <v>328.3152770996094</v>
+        <v>328.3152648925781</v>
       </c>
       <c r="K196" t="n">
-        <v>323.9980361938477</v>
+        <v>323.998030090332</v>
       </c>
     </row>
     <row r="197">
@@ -6230,16 +6230,16 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>343.685599250486</v>
+        <v>343.6855683432325</v>
       </c>
       <c r="D197" t="n">
-        <v>344.8610586187926</v>
+        <v>344.8610276058315</v>
       </c>
       <c r="E197" t="n">
-        <v>336.3142253656459</v>
+        <v>336.3141951212917</v>
       </c>
       <c r="F197" t="n">
-        <v>339.3524475097656</v>
+        <v>339.3524169921875</v>
       </c>
       <c r="G197" t="n">
         <v>55053800</v>
@@ -6251,10 +6251,10 @@
         <v>0</v>
       </c>
       <c r="J197" t="n">
-        <v>330.4191162109375</v>
+        <v>330.4190979003906</v>
       </c>
       <c r="K197" t="n">
-        <v>325.3866470336914</v>
+        <v>325.3866394042969</v>
       </c>
     </row>
     <row r="198">
@@ -6285,10 +6285,10 @@
         <v>0</v>
       </c>
       <c r="J198" t="n">
-        <v>329.7357727050781</v>
+        <v>329.7357543945312</v>
       </c>
       <c r="K198" t="n">
-        <v>326.0963912963867</v>
+        <v>326.0963836669922</v>
       </c>
     </row>
     <row r="199">
@@ -6319,10 +6319,10 @@
         <v>0</v>
       </c>
       <c r="J199" t="n">
-        <v>330.3613403320313</v>
+        <v>330.3613220214844</v>
       </c>
       <c r="K199" t="n">
-        <v>326.7966720581055</v>
+        <v>326.7966659545899</v>
       </c>
     </row>
     <row r="200">
@@ -6353,10 +6353,10 @@
         <v>0</v>
       </c>
       <c r="J200" t="n">
-        <v>331.9531555175781</v>
+        <v>331.9531433105469</v>
       </c>
       <c r="K200" t="n">
-        <v>327.569172668457</v>
+        <v>327.5691665649414</v>
       </c>
     </row>
     <row r="201">
@@ -6387,10 +6387,10 @@
         <v>0</v>
       </c>
       <c r="J201" t="n">
-        <v>333.4632873535156</v>
+        <v>333.46328125</v>
       </c>
       <c r="K201" t="n">
-        <v>328.8003921508789</v>
+        <v>328.8003845214844</v>
       </c>
     </row>
     <row r="202">
@@ -6424,7 +6424,7 @@
         <v>334.5391052246094</v>
       </c>
       <c r="K202" t="n">
-        <v>330.1506500244141</v>
+        <v>330.1506423950195</v>
       </c>
     </row>
     <row r="203">
@@ -6458,7 +6458,7 @@
         <v>338.6093017578125</v>
       </c>
       <c r="K203" t="n">
-        <v>331.5930511474609</v>
+        <v>331.5930435180664</v>
       </c>
     </row>
     <row r="204">
@@ -6492,7 +6492,7 @@
         <v>343.1895141601562</v>
       </c>
       <c r="K204" t="n">
-        <v>332.8651107788086</v>
+        <v>332.865103149414</v>
       </c>
     </row>
     <row r="205">
@@ -6502,16 +6502,16 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>352.0829877799089</v>
+        <v>352.0830180338521</v>
       </c>
       <c r="D205" t="n">
-        <v>356.1571654031082</v>
+        <v>356.1571960071392</v>
       </c>
       <c r="E205" t="n">
-        <v>351.9833684659862</v>
+        <v>351.9833987113694</v>
       </c>
       <c r="F205" t="n">
-        <v>355.1510620117188</v>
+        <v>355.1510925292969</v>
       </c>
       <c r="G205" t="n">
         <v>23828300</v>
@@ -6523,10 +6523,10 @@
         <v>0</v>
       </c>
       <c r="J205" t="n">
-        <v>347.0186462402344</v>
+        <v>347.01865234375</v>
       </c>
       <c r="K205" t="n">
-        <v>334.1954452514648</v>
+        <v>334.1954391479492</v>
       </c>
     </row>
     <row r="206">
@@ -6557,10 +6557,10 @@
         <v>0</v>
       </c>
       <c r="J206" t="n">
-        <v>351.4853088378906</v>
+        <v>351.4853149414063</v>
       </c>
       <c r="K206" t="n">
-        <v>335.7962295532226</v>
+        <v>335.796223449707</v>
       </c>
     </row>
     <row r="207">
@@ -6591,10 +6591,10 @@
         <v>0</v>
       </c>
       <c r="J207" t="n">
-        <v>354.8980590820312</v>
+        <v>354.8980651855469</v>
       </c>
       <c r="K207" t="n">
-        <v>337.3292770385742</v>
+        <v>337.3292709350586</v>
       </c>
     </row>
     <row r="208">
@@ -6625,10 +6625,10 @@
         <v>0</v>
       </c>
       <c r="J208" t="n">
-        <v>357.3624877929688</v>
+        <v>357.3624938964844</v>
       </c>
       <c r="K208" t="n">
-        <v>338.800065612793</v>
+        <v>338.8000610351563</v>
       </c>
     </row>
     <row r="209">
@@ -6659,10 +6659,10 @@
         <v>0</v>
       </c>
       <c r="J209" t="n">
-        <v>360.7234436035156</v>
+        <v>360.7234497070312</v>
       </c>
       <c r="K209" t="n">
-        <v>340.8889541625977</v>
+        <v>340.8889511108399</v>
       </c>
     </row>
     <row r="210">
@@ -6696,7 +6696,7 @@
         <v>362.7455932617187</v>
       </c>
       <c r="K210" t="n">
-        <v>342.5843704223633</v>
+        <v>342.5843688964844</v>
       </c>
     </row>
     <row r="211">
@@ -6706,16 +6706,16 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>369.5750797669642</v>
+        <v>369.5750491883937</v>
       </c>
       <c r="D211" t="n">
-        <v>370.5114466253229</v>
+        <v>370.5114159692776</v>
       </c>
       <c r="E211" t="n">
-        <v>365.9292316502895</v>
+        <v>365.9292013733758</v>
       </c>
       <c r="F211" t="n">
-        <v>368.8379211425781</v>
+        <v>368.837890625</v>
       </c>
       <c r="G211" t="n">
         <v>27683900</v>
@@ -6727,10 +6727,10 @@
         <v>0</v>
       </c>
       <c r="J211" t="n">
-        <v>364.6860534667969</v>
+        <v>364.6860473632813</v>
       </c>
       <c r="K211" t="n">
-        <v>344.4874816894531</v>
+        <v>344.4874771118164</v>
       </c>
     </row>
     <row r="212">
@@ -6761,10 +6761,10 @@
         <v>0</v>
       </c>
       <c r="J212" t="n">
-        <v>366.1245300292969</v>
+        <v>366.1245239257813</v>
       </c>
       <c r="K212" t="n">
-        <v>346.4952026367188</v>
+        <v>346.495198059082</v>
       </c>
     </row>
     <row r="213">
@@ -6795,10 +6795,10 @@
         <v>0</v>
       </c>
       <c r="J213" t="n">
-        <v>369.3606689453125</v>
+        <v>369.3606628417969</v>
       </c>
       <c r="K213" t="n">
-        <v>348.7670578002929</v>
+        <v>348.7670532226563</v>
       </c>
     </row>
     <row r="214">
@@ -6829,10 +6829,10 @@
         <v>0</v>
       </c>
       <c r="J214" t="n">
-        <v>369.5460815429688</v>
+        <v>369.5460754394531</v>
       </c>
       <c r="K214" t="n">
-        <v>350.955094909668</v>
+        <v>350.9550903320313</v>
       </c>
     </row>
     <row r="215">
@@ -6863,10 +6863,10 @@
         <v>0</v>
       </c>
       <c r="J215" t="n">
-        <v>371.8423828125</v>
+        <v>371.8423767089844</v>
       </c>
       <c r="K215" t="n">
-        <v>353.3899444580078</v>
+        <v>353.38994140625</v>
       </c>
     </row>
     <row r="216">
@@ -6900,7 +6900,7 @@
         <v>372.55107421875</v>
       </c>
       <c r="K216" t="n">
-        <v>355.5464309692383</v>
+        <v>355.5464294433594</v>
       </c>
     </row>
     <row r="217">
@@ -7206,7 +7206,7 @@
         <v>374.0942077636719</v>
       </c>
       <c r="K225" t="n">
-        <v>371.4791458129883</v>
+        <v>371.4791442871094</v>
       </c>
     </row>
     <row r="226">
@@ -7240,7 +7240,7 @@
         <v>372.0879150390625</v>
       </c>
       <c r="K226" t="n">
-        <v>371.9283264160156</v>
+        <v>371.9283248901367</v>
       </c>
     </row>
     <row r="227">
@@ -7274,7 +7274,7 @@
         <v>370.4988525390625</v>
       </c>
       <c r="K227" t="n">
-        <v>372.3518264770508</v>
+        <v>372.3518249511719</v>
       </c>
       <c r="M227" t="n">
         <v>368.5185313541908</v>
@@ -7317,7 +7317,7 @@
         <v>370.4429565429688</v>
       </c>
       <c r="K228" t="n">
-        <v>373.0640396118164</v>
+        <v>373.0640380859375</v>
       </c>
     </row>
     <row r="229">
@@ -7351,7 +7351,7 @@
         <v>370.8741516113281</v>
       </c>
       <c r="K229" t="n">
-        <v>373.1827575683594</v>
+        <v>373.1827560424805</v>
       </c>
     </row>
     <row r="230">
@@ -7385,7 +7385,7 @@
         <v>371.2454711914062</v>
       </c>
       <c r="K230" t="n">
-        <v>373.6041152954102</v>
+        <v>373.6041137695312</v>
       </c>
     </row>
     <row r="231">

</xml_diff>